<commit_message>
feat: Update case study file name in main_2.py
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/ranking_of_23_alternatives.xlsx
+++ b/Repo/Articulo1/output/ranking_of_23_alternatives.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08/05/24</t>
+          <t>08/14/24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>172.1187226027397</v>
+        <v>151.6650924657534</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -591,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>86.05936130136985</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -620,13 +620,13 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>86.05936130136985</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G4" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H4" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -649,16 +649,16 @@
         <v>250</v>
       </c>
       <c r="F5" t="n">
-        <v>86.05936130136985</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I5" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="6">
@@ -678,10 +678,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>86.05936130136985</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G6" t="n">
-        <v>261.5297621917808</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -707,16 +707,16 @@
         <v>250</v>
       </c>
       <c r="F7" t="n">
-        <v>86.05936130136985</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G7" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="8">
@@ -736,7 +736,7 @@
         <v>500</v>
       </c>
       <c r="F8" t="n">
-        <v>86.05936130136985</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="9">
@@ -765,13 +765,13 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G9" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H9" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -794,16 +794,16 @@
         <v>250</v>
       </c>
       <c r="F10" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I10" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="11">
@@ -823,13 +823,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G11" t="n">
-        <v>261.5297621917808</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H11" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -852,16 +852,16 @@
         <v>250</v>
       </c>
       <c r="F12" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G12" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H12" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I12" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="13">
@@ -881,16 +881,16 @@
         <v>500</v>
       </c>
       <c r="F13" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I13" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="14">
@@ -910,16 +910,16 @@
         <v>250</v>
       </c>
       <c r="F14" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G14" t="n">
-        <v>261.5297621917808</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="15">
@@ -939,16 +939,16 @@
         <v>500</v>
       </c>
       <c r="F15" t="n">
-        <v>51.63561678082191</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G15" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="16">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1000,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>261.5297621917808</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H17" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1029,13 +1029,13 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H18" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I18" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="19">
@@ -1061,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I19" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="20">
@@ -1087,13 +1087,13 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>261.5297621917808</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H20" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I20" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="21">
@@ -1116,13 +1116,13 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>156.9178573150685</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H21" t="n">
-        <v>22.12631772356879</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I21" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="22">
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>523.0595243835617</v>
+        <v>598.2288367089051</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1174,13 +1174,13 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>261.5297621917808</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="24">
@@ -1209,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>83.61212608909143</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
   </sheetData>
@@ -1298,22 +1298,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06752472190599633</v>
+        <v>0.05105381942179634</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05543633785513077</v>
+        <v>0.04648895864869391</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0003606650276771675</v>
+        <v>0.0003132571709710378</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3335777751906615</v>
+        <v>0.337317112252536</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01375871433942304</v>
+        <v>0.01325594133208014</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04882927641566125</v>
+        <v>0.04907417715737528</v>
       </c>
       <c r="H2" t="n">
         <v>0.1054275896195656</v>
@@ -1339,22 +1339,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04461303083397835</v>
+        <v>0.02864461303828462</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1595894574617401</v>
+        <v>0.1338318506553309</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002908842794522444</v>
+        <v>0.0002868799774037635</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2909970505118693</v>
+        <v>0.3185780114171409</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01439824439776368</v>
+        <v>0.01352407287266085</v>
       </c>
       <c r="G3" t="n">
-        <v>0.100299089855954</v>
+        <v>0.07158646518654961</v>
       </c>
       <c r="H3" t="n">
         <v>0.1370558665054353</v>
@@ -1372,7 +1372,7 @@
         <v>0.292167395960639</v>
       </c>
       <c r="M3" t="n">
-        <v>0.06743672162883274</v>
+        <v>0.02176015267698255</v>
       </c>
     </row>
     <row r="4">
@@ -1380,22 +1380,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1523449872176691</v>
+        <v>0.1343679182096427</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09449375770760927</v>
+        <v>0.0792425431511828</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0001206063852552448</v>
+        <v>9.280462970036676e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2403406994927218</v>
+        <v>0.2428453831252206</v>
       </c>
       <c r="F4" t="n">
-        <v>0.227242678406549</v>
+        <v>0.2504348589023849</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2054533122268991</v>
+        <v>0.2135149499256719</v>
       </c>
       <c r="H4" t="n">
         <v>0.1887153854190225</v>
@@ -1413,7 +1413,7 @@
         <v>0.2373860092180192</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1870003551461101</v>
+        <v>0.1535298151868136</v>
       </c>
     </row>
     <row r="5">
@@ -1421,22 +1421,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1594210927570168</v>
+        <v>0.1582098803580134</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2713339955764505</v>
+        <v>0.2745144833078922</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2438672651141936</v>
+        <v>0.2764829718992348</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2157324760159336</v>
+        <v>0.2053688436063582</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01902692605998813</v>
+        <v>0.01954455990001895</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1253470062179139</v>
+        <v>0.1210818497814034</v>
       </c>
       <c r="H5" t="n">
         <v>0.131784487024457</v>
@@ -1454,7 +1454,7 @@
         <v>0.2556464714655591</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1311447587499258</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="6">
@@ -1462,22 +1462,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2133163342450536</v>
+        <v>0.201732341894174</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02939805795347844</v>
+        <v>0.02465323564703465</v>
       </c>
       <c r="D6" t="n">
-        <v>9.171206722791621e-05</v>
+        <v>6.55800754856158e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2371485834021518</v>
+        <v>0.2339296001838458</v>
       </c>
       <c r="F6" t="n">
-        <v>0.284797882072781</v>
+        <v>0.2901267625073597</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2212229148502462</v>
+        <v>0.2327731670169077</v>
       </c>
       <c r="H6" t="n">
         <v>0.2403749043326096</v>
@@ -1495,7 +1495,7 @@
         <v>0.1826046224753994</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1992731035044074</v>
+        <v>0.2196154923330204</v>
       </c>
     </row>
     <row r="7">
@@ -1503,22 +1503,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2563026465044415</v>
+        <v>0.2608151153108446</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2062382958223197</v>
+        <v>0.219925175803744</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1432175578354095</v>
+        <v>0.1462481826110516</v>
       </c>
       <c r="E7" t="n">
-        <v>0.216897877822429</v>
+        <v>0.2081180428951416</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1897214136107297</v>
+        <v>0.187043742366802</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1868035335146652</v>
+        <v>0.1951717774915859</v>
       </c>
       <c r="H7" t="n">
         <v>0.1834440059380442</v>
@@ -1536,7 +1536,7 @@
         <v>0.2008650847229393</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1832721278091045</v>
+        <v>0.2125119134690355</v>
       </c>
     </row>
     <row r="8">
@@ -1544,22 +1544,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1485704228760366</v>
+        <v>0.1550922228920195</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2053983513093632</v>
+        <v>0.2192207976424002</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2756667399394618</v>
+        <v>0.2875077447743895</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2275147047168632</v>
+        <v>0.2085019999904916</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01930610288185714</v>
+        <v>0.01967519117641872</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1025069243695791</v>
+        <v>0.1138679457392692</v>
       </c>
       <c r="H8" t="n">
         <v>0.1265131075434787</v>
@@ -1577,7 +1577,7 @@
         <v>0.2191255469704793</v>
       </c>
       <c r="M8" t="n">
-        <v>0.06370834190158246</v>
+        <v>0.08074291175723833</v>
       </c>
     </row>
     <row r="9">
@@ -1585,22 +1585,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1388400428364698</v>
+        <v>0.1241568791569281</v>
       </c>
       <c r="C9" t="n">
-        <v>0.146570317510914</v>
+        <v>0.1229139891545013</v>
       </c>
       <c r="D9" t="n">
-        <v>8.478333138121014e-05</v>
+        <v>6.402819946062528e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2264282017632758</v>
+        <v>0.2305138779719656</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2591003560633767</v>
+        <v>0.2813947124262458</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2288260087979832</v>
+        <v>0.2349807500016487</v>
       </c>
       <c r="H9" t="n">
         <v>0.2045295238619573</v>
@@ -1618,7 +1618,7 @@
         <v>0.2373860092180192</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1870003551461101</v>
+        <v>0.1535298151868136</v>
       </c>
     </row>
     <row r="10">
@@ -1626,22 +1626,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1459161483758175</v>
+        <v>0.1479988413052988</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3234105553797552</v>
+        <v>0.3181859293112107</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2971317190616684</v>
+        <v>0.3279144740007727</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1899555632804455</v>
+        <v>0.1807955895039561</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02017928092552544</v>
+        <v>0.02071566206242945</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1420841797339283</v>
+        <v>0.1344919349301618</v>
       </c>
       <c r="H10" t="n">
         <v>0.1475986254673919</v>
@@ -1659,7 +1659,7 @@
         <v>0.2556464714655591</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1311447587499258</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="11">
@@ -1667,22 +1667,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2106615252554064</v>
+        <v>0.1946389603074533</v>
       </c>
       <c r="C11" t="n">
-        <v>0.08147461775678311</v>
+        <v>0.06832468165035317</v>
       </c>
       <c r="D11" t="n">
-        <v>5.933228237311547e-05</v>
+        <v>4.321382673545467e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2198713783413997</v>
+        <v>0.2227665878359201</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2949455592942117</v>
+        <v>0.3082199173400735</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2441531430550407</v>
+        <v>0.2500593571737579</v>
       </c>
       <c r="H11" t="n">
         <v>0.2561890427755445</v>
@@ -1700,7 +1700,7 @@
         <v>0.1826046224753994</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2667095965478731</v>
+        <v>0.2413763058080368</v>
       </c>
     </row>
     <row r="12">
@@ -1708,22 +1708,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2536483720042224</v>
+        <v>0.2537221923380495</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2583148556256243</v>
+        <v>0.2635966218070625</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1487829798774958</v>
+        <v>0.1560136616589028</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1976745010566126</v>
+        <v>0.1949105836758716</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1968259133787227</v>
+        <v>0.1987463283918775</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2099193129698392</v>
+        <v>0.2104285616761434</v>
       </c>
       <c r="H12" t="n">
         <v>0.199258144380979</v>
@@ -1741,7 +1741,7 @@
         <v>0.2008650847229393</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2507086208525702</v>
+        <v>0.2342719927240143</v>
       </c>
     </row>
     <row r="13">
@@ -1749,22 +1749,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1459161483758175</v>
+        <v>0.1479988413052988</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2574749111126678</v>
+        <v>0.2628922436457187</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2971317190616684</v>
+        <v>0.3279144740007727</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1899555632804455</v>
+        <v>0.1807955895039561</v>
       </c>
       <c r="F13" t="n">
-        <v>0.02017928092552544</v>
+        <v>0.02071566206242945</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1420841797339283</v>
+        <v>0.1344919349301618</v>
       </c>
       <c r="H13" t="n">
         <v>0.1423272459864136</v>
@@ -1782,7 +1782,7 @@
         <v>0.2191255469704793</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1311447587499258</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="14">
@@ -1790,22 +1790,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.3146191845421787</v>
+        <v>0.3210866160225808</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1932191558714935</v>
+        <v>0.2090073143029144</v>
       </c>
       <c r="D14" t="n">
-        <v>0.117852347103902</v>
+        <v>0.1174943068876201</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2037480690044272</v>
+        <v>0.1993917452735499</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2535693528989286</v>
+        <v>0.2442467444714547</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2228057346257508</v>
+        <v>0.2270745225679251</v>
       </c>
       <c r="H14" t="n">
         <v>0.2509176632945662</v>
@@ -1823,7 +1823,7 @@
         <v>0.1460836979803195</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2629813692108675</v>
+        <v>0.3003584040902587</v>
       </c>
     </row>
     <row r="15">
@@ -1831,22 +1831,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2427977021232421</v>
+        <v>0.2506045348720556</v>
       </c>
       <c r="C15" t="n">
-        <v>0.192379211358537</v>
+        <v>0.2083029361415706</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1600490733470475</v>
+        <v>0.1594645026543197</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2031497527032081</v>
+        <v>0.1964164933225691</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2104532945358148</v>
+        <v>0.2027833650702837</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2030599264628946</v>
+        <v>0.2084029306405552</v>
       </c>
       <c r="H15" t="n">
         <v>0.1939867649000008</v>
@@ -1864,7 +1864,7 @@
         <v>0.1643441602278594</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1832721278091045</v>
+        <v>0.2125119134690355</v>
       </c>
     </row>
     <row r="16">
@@ -1872,22 +1872,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.01085061643203737</v>
+        <v>0.003117666638272399</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2637425770683495</v>
+        <v>0.221174742661968</v>
       </c>
       <c r="D16" t="n">
-        <v>1.947591149456704e-05</v>
+        <v>1.691588723243604e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1253834270796475</v>
+        <v>0.1267889490619072</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0168856948711101</v>
+        <v>0.01626865527118926</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3004878548656077</v>
+        <v>0.3019949363530786</v>
       </c>
       <c r="H16" t="n">
         <v>0.168684143391305</v>
@@ -1905,7 +1905,7 @@
         <v>0.292167395960639</v>
       </c>
       <c r="M16" t="n">
-        <v>0.06743672162883274</v>
+        <v>0.02176015267698255</v>
       </c>
     </row>
     <row r="17">
@@ -1913,22 +1913,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1904043759283216</v>
+        <v>0.1793226310353442</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1335511775600878</v>
+        <v>0.1119961276536717</v>
       </c>
       <c r="D17" t="n">
-        <v>4.478738313695066e-06</v>
+        <v>3.129489259148024e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1991735792618647</v>
+        <v>0.2057627736132758</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3461317290135035</v>
+        <v>0.3520042915599342</v>
       </c>
       <c r="G17" t="n">
-        <v>0.279709119701651</v>
+        <v>0.2798926819487377</v>
       </c>
       <c r="H17" t="n">
         <v>0.2720031812184793</v>
@@ -1946,7 +1946,7 @@
         <v>0.1826046224753994</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2667095965478731</v>
+        <v>0.2413763058080368</v>
       </c>
     </row>
     <row r="18">
@@ -1954,22 +1954,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2333906881877094</v>
+        <v>0.2384058630659404</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3103914154289291</v>
+        <v>0.307268067810381</v>
       </c>
       <c r="D18" t="n">
-        <v>0.177961501946634</v>
+        <v>0.1798785327149893</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1709573769906373</v>
+        <v>0.173081542406469</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2328149577140153</v>
+        <v>0.2271779123780381</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2415877279941256</v>
+        <v>0.2351596820014379</v>
       </c>
       <c r="H18" t="n">
         <v>0.2150722828239139</v>
@@ -1987,7 +1987,7 @@
         <v>0.2008650847229393</v>
       </c>
       <c r="M18" t="n">
-        <v>0.2507086208525702</v>
+        <v>0.2342719927240143</v>
       </c>
     </row>
     <row r="19">
@@ -1995,22 +1995,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1256584645593045</v>
+        <v>0.1326825120331897</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3095514709159725</v>
+        <v>0.3065636896490372</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4420563044730739</v>
+        <v>0.4548995333973023</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1198204004591918</v>
+        <v>0.1201240522613247</v>
       </c>
       <c r="F19" t="n">
-        <v>0.02331451668581615</v>
+        <v>0.02360726490118639</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1876231141388111</v>
+        <v>0.1676019047645725</v>
       </c>
       <c r="H19" t="n">
         <v>0.1581413844293484</v>
@@ -2028,7 +2028,7 @@
         <v>0.2191255469704793</v>
       </c>
       <c r="M19" t="n">
-        <v>0.1311447587499258</v>
+        <v>0.1025029910122171</v>
       </c>
     </row>
     <row r="20">
@@ -2036,22 +2036,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3052121706066459</v>
+        <v>0.3088879442164656</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2452957156747982</v>
+        <v>0.2526787603062329</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1272721962967742</v>
+        <v>0.1282058225918037</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1807737092732757</v>
+        <v>0.1830328459989394</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2730266765592981</v>
+        <v>0.2654249183778162</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2519455443513431</v>
+        <v>0.2478532841636987</v>
       </c>
       <c r="H20" t="n">
         <v>0.2667318017375011</v>
@@ -2069,7 +2069,7 @@
         <v>0.1460836979803195</v>
       </c>
       <c r="M20" t="n">
-        <v>0.3304178622543332</v>
+        <v>0.3221184833452375</v>
       </c>
     </row>
     <row r="21">
@@ -2077,22 +2077,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2333906881877094</v>
+        <v>0.2384058630659404</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2444557711618417</v>
+        <v>0.251974382144889</v>
       </c>
       <c r="D21" t="n">
-        <v>0.177961501946634</v>
+        <v>0.1798785327149893</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1709573769906373</v>
+        <v>0.173081542406469</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2328149577140153</v>
+        <v>0.2271779123780381</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2415877279941256</v>
+        <v>0.2351596820014379</v>
       </c>
       <c r="H21" t="n">
         <v>0.2098009033429356</v>
@@ -2110,7 +2110,7 @@
         <v>0.1643441602278594</v>
       </c>
       <c r="M21" t="n">
-        <v>0.2507086208525702</v>
+        <v>0.2342719927240143</v>
       </c>
     </row>
     <row r="22">
@@ -2118,22 +2118,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3591074120946828</v>
+        <v>0.3524104057526262</v>
       </c>
       <c r="C22" t="n">
-        <v>0.003359778051826108</v>
+        <v>0.002817512645375388</v>
       </c>
       <c r="D22" t="n">
-        <v>3.20991874632679e-06</v>
+        <v>2.787988821642237e-06</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2054164509982111</v>
+        <v>0.2077191264324403</v>
       </c>
       <c r="F22" t="n">
-        <v>0.3739868715897718</v>
+        <v>0.360320587117451</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2779512657506871</v>
+        <v>0.2793453161265977</v>
       </c>
       <c r="H22" t="n">
         <v>0.3753222190456537</v>
@@ -2151,7 +2151,7 @@
         <v>0.07304184899015975</v>
       </c>
       <c r="M22" t="n">
-        <v>0.3985462070088148</v>
+        <v>0.4392317188860784</v>
       </c>
     </row>
     <row r="23">
@@ -2159,22 +2159,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2943620352150939</v>
+        <v>0.3057702867504717</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1793600714077108</v>
+        <v>0.1973850746407409</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1354300785578041</v>
+        <v>0.1305276847430411</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1843241576541362</v>
+        <v>0.1840517451307557</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2894470767272932</v>
+        <v>0.2699379638586017</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2488332413945726</v>
+        <v>0.2468725556078921</v>
       </c>
       <c r="H23" t="n">
         <v>0.2614604222565228</v>
@@ -2192,7 +2192,7 @@
         <v>0.1095627734852396</v>
       </c>
       <c r="M23" t="n">
-        <v>0.2629813692108675</v>
+        <v>0.3003584040902587</v>
       </c>
     </row>
     <row r="24">
@@ -2200,22 +2200,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1148083291677525</v>
+        <v>0.1295648545671958</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1776801823817978</v>
+        <v>0.1959763183180532</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5590307928996097</v>
+        <v>0.4855486150051087</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1183482793620165</v>
+        <v>0.1196749388104001</v>
       </c>
       <c r="F24" t="n">
-        <v>0.02501584425349644</v>
+        <v>0.02410171151287297</v>
       </c>
       <c r="G24" t="n">
-        <v>0.157756123804444</v>
+        <v>0.1585473415853663</v>
       </c>
       <c r="H24" t="n">
         <v>0.1475986254673919</v>
@@ -2233,7 +2233,7 @@
         <v>0.1460836979803195</v>
       </c>
       <c r="M24" t="n">
-        <v>0.06370834190158246</v>
+        <v>0.08074291175723833</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7410720122893284</v>
+        <v>0.7530530141799295</v>
       </c>
     </row>
     <row r="3">
@@ -2395,7 +2395,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7228736793549534</v>
+        <v>0.7217855148090941</v>
       </c>
     </row>
     <row r="4">
@@ -2403,23 +2403,23 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6765701989916362</v>
+        <v>0.7210686234971996</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6565509223778222</v>
+        <v>0.6860518801332826</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6343244500376095</v>
+        <v>0.6821010285108894</v>
       </c>
     </row>
     <row r="7">
@@ -2427,23 +2427,23 @@
         <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6280838619445697</v>
+        <v>0.6736130465966271</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.626905360649054</v>
+        <v>0.6670106954526674</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6142595696228971</v>
+        <v>0.6633767066819743</v>
       </c>
     </row>
     <row r="10">
@@ -2451,39 +2451,39 @@
         <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6010545507033288</v>
+        <v>0.6582670122009904</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5358215326172919</v>
+        <v>0.5885289903265453</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5257158885136879</v>
+        <v>0.5713649193293828</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5208283783699974</v>
+        <v>0.5206271658452135</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5074831157873442</v>
+        <v>0.5073357613457374</v>
       </c>
     </row>
     <row r="15">
@@ -2491,7 +2491,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="n">
-        <v>0.478958554211466</v>
+        <v>0.4790585469410924</v>
       </c>
     </row>
     <row r="16">
@@ -2499,7 +2499,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4232862147219187</v>
+        <v>0.4733654728337816</v>
       </c>
     </row>
     <row r="17">
@@ -2507,7 +2507,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.4044609886666365</v>
+        <v>0.4582814329096751</v>
       </c>
     </row>
     <row r="18">
@@ -2515,7 +2515,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.402138189372063</v>
+        <v>0.4552435577376918</v>
       </c>
     </row>
     <row r="19">
@@ -2523,31 +2523,31 @@
         <v>9</v>
       </c>
       <c r="B19" t="n">
-        <v>0.372881683040477</v>
+        <v>0.4339811154156679</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3728506259093026</v>
+        <v>0.4180925665283239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3608594309629752</v>
+        <v>0.3538192547620688</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3549446995830375</v>
+        <v>0.3439000330375241</v>
       </c>
     </row>
     <row r="23">
@@ -2555,7 +2555,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="n">
-        <v>0.266621649332517</v>
+        <v>0.304685973317776</v>
       </c>
     </row>
     <row r="24">
@@ -2563,7 +2563,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="n">
-        <v>0.201842076308632</v>
+        <v>0.1872750736235602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>